<commit_message>
Built first ML model with DOPPIO data
</commit_message>
<xml_diff>
--- a/data/q2a_sites.xlsx
+++ b/data/q2a_sites.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henrysun_1/Desktop/Duke/2024-2025/Summer 2024/fishics/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB90B927-42FE-F842-9A8A-5CE2522C5DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F75039-D0BF-9A48-8059-03946B48DB15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{F88DDB59-38D0-AA46-82AC-51FC22E0688B}"/>
   </bookViews>
@@ -419,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3421C3EA-C4AE-214C-86FC-F1644C7B3181}">
-  <dimension ref="A2:D23"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection sqref="A1:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -433,311 +433,311 @@
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B2">
+        <v>-74.204406739999996</v>
+      </c>
+      <c r="C2">
+        <v>39.183304249999999</v>
+      </c>
+      <c r="D2">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>-74.204406739999996</v>
+        <v>-74.207153320000003</v>
       </c>
       <c r="C3">
-        <v>39.183304249999999</v>
+        <v>39.104488809999999</v>
       </c>
       <c r="D3">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4">
-        <v>-74.207153320000003</v>
+        <v>-74.092545110000003</v>
       </c>
       <c r="C4">
-        <v>39.104488809999999</v>
+        <v>39.272987550000003</v>
       </c>
       <c r="D4">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5">
-        <v>-74.092545110000003</v>
+        <v>-74.050598140000005</v>
       </c>
       <c r="C5">
-        <v>39.272987550000003</v>
+        <v>39.325799420000003</v>
       </c>
       <c r="D5">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6">
-        <v>-74.050598140000005</v>
+        <v>-74.130249019999994</v>
       </c>
       <c r="C6">
-        <v>39.325799420000003</v>
+        <v>39.21523131</v>
       </c>
       <c r="D6">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7">
-        <v>-74.130249019999994</v>
+        <v>-74.053344730000006</v>
       </c>
       <c r="C7">
-        <v>39.21523131</v>
+        <v>39.217359260000002</v>
       </c>
       <c r="D7">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8">
-        <v>-74.053344730000006</v>
+        <v>-74.440612790000003</v>
       </c>
       <c r="C8">
         <v>39.217359260000002</v>
       </c>
       <c r="D8">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <v>-74.440612790000003</v>
+        <v>-74.286804200000006</v>
       </c>
       <c r="C9">
-        <v>39.217359260000002</v>
+        <v>39.404366619999998</v>
       </c>
       <c r="D9">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10">
-        <v>-74.286804200000006</v>
+        <v>-74.130249019999994</v>
       </c>
       <c r="C10">
-        <v>39.404366619999998</v>
+        <v>39.550647619999999</v>
       </c>
       <c r="D10">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11">
-        <v>-74.130249019999994</v>
+        <v>-74.004084370000001</v>
       </c>
       <c r="C11">
-        <v>39.550647619999999</v>
+        <v>39.47223048</v>
       </c>
       <c r="D11">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12">
-        <v>-74.004084370000001</v>
+        <v>-74.127502440000001</v>
       </c>
       <c r="C12">
-        <v>39.47223048</v>
+        <v>39.068246729999998</v>
       </c>
       <c r="D12">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13">
-        <v>-74.127502440000001</v>
+        <v>-73.972531529999998</v>
       </c>
       <c r="C13">
-        <v>39.068246729999998</v>
+        <v>38.991053729999997</v>
       </c>
       <c r="D13">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14">
-        <v>-73.972531529999998</v>
+        <v>-73.973693850000004</v>
       </c>
       <c r="C14">
-        <v>38.991053729999997</v>
+        <v>39.21523131</v>
       </c>
       <c r="D14">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15">
-        <v>-73.973693850000004</v>
+        <v>-73.896789549999994</v>
       </c>
       <c r="C15">
-        <v>39.21523131</v>
+        <v>39.364032340000001</v>
       </c>
       <c r="D15">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16">
-        <v>-73.896789549999994</v>
+        <v>-73.739540340000005</v>
       </c>
       <c r="C16">
-        <v>39.364032340000001</v>
+        <v>39.28829983</v>
       </c>
       <c r="D16">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17">
-        <v>-73.739540340000005</v>
+        <v>-73.891296389999994</v>
       </c>
       <c r="C17">
-        <v>39.28829983</v>
+        <v>39.47648555</v>
       </c>
       <c r="D17">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18">
-        <v>-73.891296389999994</v>
+        <v>-73.740234380000004</v>
       </c>
       <c r="C18">
-        <v>39.47648555</v>
+        <v>39.47224533</v>
       </c>
       <c r="D18">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19">
-        <v>-73.740234380000004</v>
+        <v>-73.972531529999998</v>
       </c>
       <c r="C19">
-        <v>39.47224533</v>
+        <v>39.73416898</v>
       </c>
       <c r="D19">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20">
-        <v>-73.972531529999998</v>
+        <v>-73.896789549999994</v>
       </c>
       <c r="C20">
-        <v>39.73416898</v>
+        <v>39.660685020000003</v>
       </c>
       <c r="D20">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21">
-        <v>-73.896789549999994</v>
+        <v>-73.740234380000004</v>
       </c>
       <c r="C21">
-        <v>39.660685020000003</v>
+        <v>39.662799409999998</v>
       </c>
       <c r="D21">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B22">
-        <v>-73.740234380000004</v>
+        <v>-73.973693850000004</v>
       </c>
       <c r="C22">
-        <v>39.662799409999998</v>
+        <v>39.582407119999999</v>
       </c>
       <c r="D22">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>21</v>
-      </c>
-      <c r="B23">
-        <v>-73.973693850000004</v>
-      </c>
-      <c r="C23">
-        <v>39.582407119999999</v>
-      </c>
-      <c r="D23">
         <v>31</v>
       </c>
     </row>

</xml_diff>